<commit_message>
Ajout du rapport et mise à jour de documents
</commit_message>
<xml_diff>
--- a/BottomUp.xlsx
+++ b/BottomUp.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25007"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25306"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="100" windowWidth="14800" windowHeight="8020"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15480"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -19,10 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="33">
-  <si>
-    <t>Identifiant</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="55">
   <si>
     <t>Type</t>
   </si>
@@ -33,6 +30,9 @@
     <t>Criticité</t>
   </si>
   <si>
+    <t>Flexibilité</t>
+  </si>
+  <si>
     <t>Expression de la fonction</t>
   </si>
   <si>
@@ -42,89 +42,155 @@
     <t>Service</t>
   </si>
   <si>
-    <t>Détecter l'individu via une caméra</t>
-  </si>
-  <si>
-    <t>Détecter les mouvements des yeux</t>
+    <t>Positionner l'utilisateur pour l'acquisition vidéo</t>
+  </si>
+  <si>
+    <t>Acquérir les données nécessaires à la détection du mouvement de l'oeil</t>
   </si>
   <si>
     <t>1.1.2</t>
   </si>
   <si>
-    <t>Détecter l'oeil (pupille)</t>
+    <t>Filmer le visage de l'utilisateur</t>
   </si>
   <si>
     <t>1.1.3</t>
   </si>
   <si>
+    <t>Acquérir les données nécessaires à l'estimation de la distance de l'utilisateur à l'interface</t>
+  </si>
+  <si>
+    <t>1.1.4</t>
+  </si>
+  <si>
     <t>Contrainte</t>
   </si>
   <si>
-    <t>Estimer la distance de l'individu à l'interface</t>
-  </si>
-  <si>
-    <t>1.1.4</t>
-  </si>
-  <si>
-    <t>Relayer les informations de positionnement/localisation au système embarqué</t>
-  </si>
-  <si>
-    <t>1.2.1.1</t>
-  </si>
-  <si>
-    <t>Compresser le flux vidéo</t>
-  </si>
-  <si>
-    <t>Transférer des informations du système embarqué à l'ordinateur</t>
-  </si>
-  <si>
-    <t>1.2.1.2</t>
-  </si>
-  <si>
-    <t>Transmettre le signal compressé à l'ordinateur via un  réseau sans fil</t>
-  </si>
-  <si>
-    <t>1.2.2.1</t>
-  </si>
-  <si>
-    <t>Analyser le mouvement de la pupille</t>
-  </si>
-  <si>
-    <t>Traiter et interpréter les informations reçues (partie algorithmique)</t>
-  </si>
-  <si>
-    <t>1.2.2.2</t>
-  </si>
-  <si>
-    <t>Déduire les nouvelles coodonnées du curseur ou une action utilisateur</t>
+    <t>Etre utilisable à une distance de 50cm à 3m</t>
+  </si>
+  <si>
+    <t>1.1.5</t>
+  </si>
+  <si>
+    <t>Avoir une autonomie de Xh</t>
+  </si>
+  <si>
+    <t>1.2.1</t>
+  </si>
+  <si>
+    <t>Relayer les données à la carte de traitement</t>
+  </si>
+  <si>
+    <t>Transférer les données enregistrées</t>
+  </si>
+  <si>
+    <t>1.2.2</t>
+  </si>
+  <si>
+    <t>Transmettre le signal compressé</t>
+  </si>
+  <si>
+    <t>1.2.3</t>
+  </si>
+  <si>
+    <t>Effectuer la transmission sans fil</t>
   </si>
   <si>
     <t>1.3.1</t>
   </si>
   <si>
+    <t>Détecter l'utilisateur et ses mouvements :</t>
+  </si>
+  <si>
+    <t>Traiter les données enregistrées</t>
+  </si>
+  <si>
+    <t>1.3.1.1</t>
+  </si>
+  <si>
+    <t>Détecter le visage de l'utilisateur</t>
+  </si>
+  <si>
+    <t>1.3.1.2</t>
+  </si>
+  <si>
+    <t>Détecter les yeux de l'utilisateur</t>
+  </si>
+  <si>
+    <t>1.3.1.3</t>
+  </si>
+  <si>
+    <t>Détecter les pupilles de l'utilisateur</t>
+  </si>
+  <si>
+    <t>1.3.1.4</t>
+  </si>
+  <si>
+    <t>Détecter le mouvement des pupilles de l'utilisateur</t>
+  </si>
+  <si>
+    <t>1.3.1.5</t>
+  </si>
+  <si>
+    <t>Détecter le clignement des yeux de l'utilisateur</t>
+  </si>
+  <si>
+    <t>1.3.2</t>
+  </si>
+  <si>
+    <t>Calculer la distance entre l'utilisateur et l'interface</t>
+  </si>
+  <si>
+    <t>1.4.1</t>
+  </si>
+  <si>
+    <t>Analyser le mouvement de la pupille à l'aide de la distance utilisateur-IHM</t>
+  </si>
+  <si>
+    <t>Interpréter les données pour déduire l'action à exécuter</t>
+  </si>
+  <si>
+    <t>1.4.2</t>
+  </si>
+  <si>
+    <t>Déduire l'action à effectuer</t>
+  </si>
+  <si>
+    <t>1.5.1</t>
+  </si>
+  <si>
     <t>Afficher le curseur à l'endroit regardé par l'utilisateur</t>
   </si>
   <si>
     <t>Agir sur l'IHM</t>
   </si>
   <si>
-    <t>1.3.2</t>
+    <t>1.5.2</t>
+  </si>
+  <si>
+    <t>Actualiser l'affichage en moins de 10ms</t>
+  </si>
+  <si>
+    <t>1.5.3</t>
   </si>
   <si>
     <t>Permettre le clic gauche / la sélection</t>
   </si>
   <si>
-    <t>1.3.3</t>
+    <t>1.5.4</t>
   </si>
   <si>
     <t>Permettre à l'utilisateur de désactiver (mettre en pause) le système de détection</t>
+  </si>
+  <si>
+    <t>Id</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -137,8 +203,24 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -159,18 +241,24 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFEBDF69"/>
+        <fgColor rgb="FFFF7358"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF7358"/>
+        <fgColor rgb="FFEBCB69"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE9EB79"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -193,56 +281,138 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="13">
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -521,237 +691,458 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="11.6640625" customWidth="1"/>
-    <col min="3" max="3" width="82.5" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" customWidth="1"/>
-    <col min="5" max="5" width="42.33203125" customWidth="1"/>
+    <col min="1" max="1" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" customWidth="1"/>
+    <col min="3" max="3" width="68.1640625" customWidth="1"/>
+    <col min="4" max="5" width="7.83203125" customWidth="1"/>
+    <col min="6" max="6" width="31.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="3" t="s">
+    <row r="2" spans="1:6">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="4">
-        <v>5</v>
-      </c>
-      <c r="E2" s="5" t="s">
+      <c r="D2" s="3">
+        <v>5</v>
+      </c>
+      <c r="E2" s="3">
+        <v>5</v>
+      </c>
+      <c r="F2" s="8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:6">
+      <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="4">
-        <v>5</v>
-      </c>
-      <c r="E3" s="5"/>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="3" t="s">
+      <c r="D3" s="3">
+        <v>5</v>
+      </c>
+      <c r="E3" s="3">
+        <v>4</v>
+      </c>
+      <c r="F3" s="8"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3">
+        <v>5</v>
+      </c>
+      <c r="E4" s="3">
+        <v>5</v>
+      </c>
+      <c r="F4" s="8"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="4">
-        <v>5</v>
-      </c>
-      <c r="E4" s="5"/>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="3" t="s">
+      <c r="B5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="4">
-        <v>5</v>
-      </c>
-      <c r="E5" s="5"/>
-    </row>
-    <row r="6" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A6" s="9" t="s">
+      <c r="D5" s="3">
+        <v>5</v>
+      </c>
+      <c r="E5" s="3">
+        <v>3</v>
+      </c>
+      <c r="F5" s="8"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="9" t="s">
+      <c r="B6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="10">
-        <v>5</v>
-      </c>
-      <c r="E6" s="11" t="s">
+      <c r="D6" s="3">
+        <v>4</v>
+      </c>
+      <c r="E6" s="3">
+        <v>3</v>
+      </c>
+      <c r="F6" s="8"/>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A7" s="17" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A7" s="9" t="s">
+      <c r="B7" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="9" t="s">
+      <c r="D7" s="18">
+        <v>5</v>
+      </c>
+      <c r="E7" s="18">
+        <v>5</v>
+      </c>
+      <c r="F7" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="10">
-        <v>5</v>
-      </c>
-      <c r="E7" s="11"/>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="6" t="s">
+    </row>
+    <row r="8" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A8" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="6" t="s">
+      <c r="B8" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="7">
-        <v>5</v>
-      </c>
-      <c r="E8" s="8" t="s">
+      <c r="D8" s="18">
+        <v>5</v>
+      </c>
+      <c r="E8" s="18">
+        <v>5</v>
+      </c>
+      <c r="F8" s="20"/>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A9" s="17" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="6" t="s">
+      <c r="B9" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="6" t="s">
+      <c r="D9" s="18">
+        <v>3</v>
+      </c>
+      <c r="E9" s="18">
+        <v>3</v>
+      </c>
+      <c r="F9" s="21"/>
+    </row>
+    <row r="10" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A10" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="7">
-        <v>5</v>
-      </c>
-      <c r="E9" s="8"/>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="12" t="s">
+      <c r="B10" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="12" t="s">
+      <c r="D10" s="13">
+        <v>5</v>
+      </c>
+      <c r="E10" s="13">
+        <v>5</v>
+      </c>
+      <c r="F10" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="13">
-        <v>5</v>
-      </c>
-      <c r="E10" s="14" t="s">
+    </row>
+    <row r="11" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A11" s="12" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="12" t="s">
+      <c r="B11" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="12" t="s">
+      <c r="D11" s="13">
+        <v>5</v>
+      </c>
+      <c r="E11" s="13">
+        <v>5</v>
+      </c>
+      <c r="F11" s="15"/>
+    </row>
+    <row r="12" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A12" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="13">
-        <v>5</v>
-      </c>
-      <c r="E11" s="14"/>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="12" t="s">
+      <c r="B12" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="12" t="s">
+      <c r="D12" s="13">
+        <v>5</v>
+      </c>
+      <c r="E12" s="13">
+        <v>5</v>
+      </c>
+      <c r="F12" s="15"/>
+    </row>
+    <row r="13" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A13" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="13">
-        <v>5</v>
-      </c>
-      <c r="E12" s="14"/>
-    </row>
-    <row r="22" spans="5:5">
-      <c r="E22" s="2"/>
-    </row>
-    <row r="23" spans="5:5">
-      <c r="E23" s="2"/>
-    </row>
-    <row r="24" spans="5:5">
-      <c r="E24" s="2"/>
-    </row>
-    <row r="25" spans="5:5">
-      <c r="E25" s="2"/>
-    </row>
-    <row r="26" spans="5:5">
-      <c r="E26" s="2"/>
-    </row>
-    <row r="27" spans="5:5">
-      <c r="E27" s="2"/>
+      <c r="B13" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="13">
+        <v>5</v>
+      </c>
+      <c r="E13" s="13">
+        <v>5</v>
+      </c>
+      <c r="F13" s="15"/>
+    </row>
+    <row r="14" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A14" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="13">
+        <v>5</v>
+      </c>
+      <c r="E14" s="13">
+        <v>5</v>
+      </c>
+      <c r="F14" s="15"/>
+    </row>
+    <row r="15" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A15" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="13">
+        <v>4</v>
+      </c>
+      <c r="E15" s="13">
+        <v>3</v>
+      </c>
+      <c r="F15" s="15"/>
+    </row>
+    <row r="16" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A16" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="13">
+        <v>5</v>
+      </c>
+      <c r="E16" s="13">
+        <v>5</v>
+      </c>
+      <c r="F16" s="16"/>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" s="5">
+        <v>5</v>
+      </c>
+      <c r="E17" s="5">
+        <v>5</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" s="5">
+        <v>5</v>
+      </c>
+      <c r="E18" s="5">
+        <v>5</v>
+      </c>
+      <c r="F18" s="10"/>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D19" s="7">
+        <v>5</v>
+      </c>
+      <c r="E19" s="7">
+        <v>4</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20" s="7">
+        <v>5</v>
+      </c>
+      <c r="E20" s="7">
+        <v>2</v>
+      </c>
+      <c r="F20" s="9"/>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D21" s="7">
+        <v>5</v>
+      </c>
+      <c r="E21" s="7">
+        <v>3</v>
+      </c>
+      <c r="F21" s="9"/>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D22" s="7">
+        <v>3</v>
+      </c>
+      <c r="E22" s="7">
+        <v>2</v>
+      </c>
+      <c r="F22" s="9"/>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="F32" s="11"/>
+    </row>
+    <row r="33" spans="6:6">
+      <c r="F33" s="11"/>
+    </row>
+    <row r="34" spans="6:6">
+      <c r="F34" s="11"/>
+    </row>
+    <row r="35" spans="6:6">
+      <c r="F35" s="11"/>
+    </row>
+    <row r="36" spans="6:6">
+      <c r="F36" s="11"/>
+    </row>
+    <row r="37" spans="6:6">
+      <c r="F37" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="E2:E5"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="E10:E12"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="E22:E27"/>
+  <mergeCells count="6">
+    <mergeCell ref="F2:F6"/>
+    <mergeCell ref="F19:F22"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="F32:F37"/>
+    <mergeCell ref="F7:F9"/>
+    <mergeCell ref="F10:F16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -944,8 +1335,15 @@
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D2CF9F40-0567-4047-ADFE-957BEF6929CE}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="703c0b8e-7b07-40a3-aeff-2f8dc6e18e60"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Modif rapport et ajout de livrables
</commit_message>
<xml_diff>
--- a/BottomUp.xlsx
+++ b/BottomUp.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25306"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25317"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15480"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -72,9 +72,6 @@
     <t>1.1.5</t>
   </si>
   <si>
-    <t>Avoir une autonomie de Xh</t>
-  </si>
-  <si>
     <t>1.2.1</t>
   </si>
   <si>
@@ -184,13 +181,16 @@
   </si>
   <si>
     <t>Id</t>
+  </si>
+  <si>
+    <t>Avoir une autonomie de 3h</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -199,8 +199,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -217,6 +219,11 @@
       <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -253,7 +260,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFE9EB79"/>
+        <fgColor rgb="FFEEECE1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -319,7 +326,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -333,86 +340,121 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="23">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -683,7 +725,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -694,443 +736,444 @@
   <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.1640625" customWidth="1"/>
-    <col min="3" max="3" width="68.1640625" customWidth="1"/>
-    <col min="4" max="5" width="7.83203125" customWidth="1"/>
-    <col min="6" max="6" width="31.5" customWidth="1"/>
+    <col min="3" max="3" width="44.6640625" customWidth="1"/>
+    <col min="4" max="4" width="7.83203125" customWidth="1"/>
+    <col min="5" max="5" width="8.1640625" customWidth="1"/>
+    <col min="6" max="6" width="22.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" ht="17" customHeight="1">
+      <c r="A1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="17" customHeight="1">
+      <c r="A2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="4">
+        <v>5</v>
+      </c>
+      <c r="E2" s="4">
+        <v>5</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="17" customHeight="1">
+      <c r="A3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="4">
+        <v>5</v>
+      </c>
+      <c r="E3" s="4">
+        <v>4</v>
+      </c>
+      <c r="F3" s="6"/>
+    </row>
+    <row r="4" spans="1:6" ht="32" customHeight="1">
+      <c r="A4" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="22">
+        <v>5</v>
+      </c>
+      <c r="E4" s="22">
+        <v>5</v>
+      </c>
+      <c r="F4" s="6"/>
+    </row>
+    <row r="5" spans="1:6" ht="17" customHeight="1">
+      <c r="A5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="4">
+        <v>5</v>
+      </c>
+      <c r="E5" s="4">
+        <v>3</v>
+      </c>
+      <c r="F5" s="6"/>
+    </row>
+    <row r="6" spans="1:6" ht="17" customHeight="1">
+      <c r="A6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="D6" s="4">
+        <v>4</v>
+      </c>
+      <c r="E6" s="4">
+        <v>3</v>
+      </c>
+      <c r="F6" s="6"/>
+    </row>
+    <row r="7" spans="1:6" ht="17" customHeight="1">
+      <c r="A7" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="22">
+        <v>5</v>
+      </c>
+      <c r="E7" s="22">
+        <v>5</v>
+      </c>
+      <c r="F7" s="24" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="17" customHeight="1">
+      <c r="A8" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="22">
+        <v>5</v>
+      </c>
+      <c r="E8" s="22">
+        <v>5</v>
+      </c>
+      <c r="F8" s="25"/>
+    </row>
+    <row r="9" spans="1:6" ht="17" customHeight="1">
+      <c r="A9" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="22">
+        <v>3</v>
+      </c>
+      <c r="E9" s="22">
+        <v>3</v>
+      </c>
+      <c r="F9" s="26"/>
+    </row>
+    <row r="10" spans="1:6" ht="17" customHeight="1">
+      <c r="A10" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="8">
+        <v>5</v>
+      </c>
+      <c r="E10" s="8">
+        <v>5</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="17" customHeight="1">
+      <c r="A11" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="8">
+        <v>5</v>
+      </c>
+      <c r="E11" s="8">
+        <v>5</v>
+      </c>
+      <c r="F11" s="11"/>
+    </row>
+    <row r="12" spans="1:6" ht="17" customHeight="1">
+      <c r="A12" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="8">
+        <v>5</v>
+      </c>
+      <c r="E12" s="8">
+        <v>5</v>
+      </c>
+      <c r="F12" s="11"/>
+    </row>
+    <row r="13" spans="1:6" ht="17" customHeight="1">
+      <c r="A13" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="8">
+        <v>5</v>
+      </c>
+      <c r="E13" s="8">
+        <v>5</v>
+      </c>
+      <c r="F13" s="11"/>
+    </row>
+    <row r="14" spans="1:6" ht="17" customHeight="1">
+      <c r="A14" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="8">
+        <v>5</v>
+      </c>
+      <c r="E14" s="8">
+        <v>5</v>
+      </c>
+      <c r="F14" s="11"/>
+    </row>
+    <row r="15" spans="1:6" ht="17" customHeight="1">
+      <c r="A15" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="8">
+        <v>4</v>
+      </c>
+      <c r="E15" s="8">
+        <v>3</v>
+      </c>
+      <c r="F15" s="11"/>
+    </row>
+    <row r="16" spans="1:6" ht="17" customHeight="1">
+      <c r="A16" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="22">
+        <v>5</v>
+      </c>
+      <c r="E16" s="22">
+        <v>5</v>
+      </c>
+      <c r="F16" s="12"/>
+    </row>
+    <row r="17" spans="1:6" ht="32" customHeight="1">
+      <c r="A17" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="14">
+        <v>5</v>
+      </c>
+      <c r="E17" s="14">
+        <v>5</v>
+      </c>
+      <c r="F17" s="16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="17" customHeight="1">
+      <c r="A18" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D18" s="14">
+        <v>5</v>
+      </c>
+      <c r="E18" s="14">
+        <v>5</v>
+      </c>
+      <c r="F18" s="16"/>
+    </row>
+    <row r="19" spans="1:6" ht="17" customHeight="1">
+      <c r="A19" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" s="18">
+        <v>5</v>
+      </c>
+      <c r="E19" s="18">
+        <v>4</v>
+      </c>
+      <c r="F19" s="20" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="17" customHeight="1">
+      <c r="A20" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="D20" s="18">
+        <v>5</v>
+      </c>
+      <c r="E20" s="18">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F20" s="20"/>
+    </row>
+    <row r="21" spans="1:6" ht="17" customHeight="1">
+      <c r="A21" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="D21" s="18">
+        <v>5</v>
+      </c>
+      <c r="E21" s="18">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="3">
-        <v>5</v>
-      </c>
-      <c r="E2" s="3">
-        <v>5</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="3">
-        <v>5</v>
-      </c>
-      <c r="E3" s="3">
-        <v>4</v>
-      </c>
-      <c r="F3" s="8"/>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="3">
-        <v>5</v>
-      </c>
-      <c r="E4" s="3">
-        <v>5</v>
-      </c>
-      <c r="F4" s="8"/>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="3">
-        <v>5</v>
-      </c>
-      <c r="E5" s="3">
+      <c r="F21" s="20"/>
+    </row>
+    <row r="22" spans="1:6" ht="32" customHeight="1">
+      <c r="A22" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="D22" s="18">
         <v>3</v>
       </c>
-      <c r="F5" s="8"/>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="3">
-        <v>4</v>
-      </c>
-      <c r="E6" s="3">
-        <v>3</v>
-      </c>
-      <c r="F6" s="8"/>
-    </row>
-    <row r="7" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A7" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="18">
-        <v>5</v>
-      </c>
-      <c r="E7" s="18">
-        <v>5</v>
-      </c>
-      <c r="F7" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A8" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" s="18">
-        <v>5</v>
-      </c>
-      <c r="E8" s="18">
-        <v>5</v>
-      </c>
-      <c r="F8" s="20"/>
-    </row>
-    <row r="9" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A9" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="18">
-        <v>3</v>
-      </c>
-      <c r="E9" s="18">
-        <v>3</v>
-      </c>
-      <c r="F9" s="21"/>
-    </row>
-    <row r="10" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A10" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="13">
-        <v>5</v>
-      </c>
-      <c r="E10" s="13">
-        <v>5</v>
-      </c>
-      <c r="F10" s="14" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A11" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="B11" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" s="13">
-        <v>5</v>
-      </c>
-      <c r="E11" s="13">
-        <v>5</v>
-      </c>
-      <c r="F11" s="15"/>
-    </row>
-    <row r="12" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A12" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="D12" s="13">
-        <v>5</v>
-      </c>
-      <c r="E12" s="13">
-        <v>5</v>
-      </c>
-      <c r="F12" s="15"/>
-    </row>
-    <row r="13" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A13" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D13" s="13">
-        <v>5</v>
-      </c>
-      <c r="E13" s="13">
-        <v>5</v>
-      </c>
-      <c r="F13" s="15"/>
-    </row>
-    <row r="14" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A14" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="B14" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="D14" s="13">
-        <v>5</v>
-      </c>
-      <c r="E14" s="13">
-        <v>5</v>
-      </c>
-      <c r="F14" s="15"/>
-    </row>
-    <row r="15" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A15" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="B15" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="D15" s="13">
-        <v>4</v>
-      </c>
-      <c r="E15" s="13">
-        <v>3</v>
-      </c>
-      <c r="F15" s="15"/>
-    </row>
-    <row r="16" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A16" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="B16" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="D16" s="13">
-        <v>5</v>
-      </c>
-      <c r="E16" s="13">
-        <v>5</v>
-      </c>
-      <c r="F16" s="16"/>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D17" s="5">
-        <v>5</v>
-      </c>
-      <c r="E17" s="5">
-        <v>5</v>
-      </c>
-      <c r="F17" s="10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D18" s="5">
-        <v>5</v>
-      </c>
-      <c r="E18" s="5">
-        <v>5</v>
-      </c>
-      <c r="F18" s="10"/>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D19" s="7">
-        <v>5</v>
-      </c>
-      <c r="E19" s="7">
-        <v>4</v>
-      </c>
-      <c r="F19" s="9" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D20" s="7">
-        <v>5</v>
-      </c>
-      <c r="E20" s="7">
+      <c r="E22" s="18">
         <v>2</v>
       </c>
-      <c r="F20" s="9"/>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="D21" s="7">
-        <v>5</v>
-      </c>
-      <c r="E21" s="7">
-        <v>3</v>
-      </c>
-      <c r="F21" s="9"/>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D22" s="7">
-        <v>3</v>
-      </c>
-      <c r="E22" s="7">
-        <v>2</v>
-      </c>
-      <c r="F22" s="9"/>
+      <c r="F22" s="20"/>
     </row>
     <row r="32" spans="1:6">
-      <c r="F32" s="11"/>
+      <c r="F32" s="1"/>
     </row>
     <row r="33" spans="6:6">
-      <c r="F33" s="11"/>
+      <c r="F33" s="1"/>
     </row>
     <row r="34" spans="6:6">
-      <c r="F34" s="11"/>
+      <c r="F34" s="1"/>
     </row>
     <row r="35" spans="6:6">
-      <c r="F35" s="11"/>
+      <c r="F35" s="1"/>
     </row>
     <row r="36" spans="6:6">
-      <c r="F36" s="11"/>
+      <c r="F36" s="1"/>
     </row>
     <row r="37" spans="6:6">
-      <c r="F37" s="11"/>
+      <c r="F37" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>